<commit_message>
deleted 3-26 due to repeat of testing on 2-27
</commit_message>
<xml_diff>
--- a/capDatabase.xlsx
+++ b/capDatabase.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Date Created</t>
   </si>
@@ -61,24 +61,9 @@
     <t>0x0003</t>
   </si>
   <si>
-    <t>Buck Supply</t>
-  </si>
-  <si>
     <t>Test Type</t>
   </si>
   <si>
-    <t>4294a_measurement</t>
-  </si>
-  <si>
-    <t>Baseline measurement</t>
-  </si>
-  <si>
-    <t>Measured an Al cap to check what the data was supposed to look like for Ti caps</t>
-  </si>
-  <si>
-    <t>1uF 50V Al-elecrolytic</t>
-  </si>
-  <si>
     <t>leakage current measurements</t>
   </si>
   <si>
@@ -86,6 +71,18 @@
   </si>
   <si>
     <t>Tant - TAP475K006SCS</t>
+  </si>
+  <si>
+    <t>buck filtering</t>
+  </si>
+  <si>
+    <t>The capacitors were put in a low power buck supply to test for degredation</t>
+  </si>
+  <si>
+    <t>leakage</t>
+  </si>
+  <si>
+    <t>Measure leakage of tant and ti capacitors</t>
   </si>
 </sst>
 </file>
@@ -134,8 +131,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -143,9 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H8" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -563,7 +568,9 @@
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -571,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -584,16 +591,18 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <f>SUM(D45)</f>
-        <v>0</v>
+      <c r="A2" s="1">
+        <v>40981</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="1">
         <v>40981</v>
       </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
@@ -603,62 +612,48 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>40994</v>
+        <v>40995</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40995</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>40995</v>
+        <v>41011</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41011</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>40995</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>41011</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1">
-        <v>41011</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data from 1st batch of caps from Evens
</commit_message>
<xml_diff>
--- a/capDatabase.xlsx
+++ b/capDatabase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Date Created</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>dcFebSummit</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>Evens</t>
+  </si>
+  <si>
+    <t>100V</t>
+  </si>
+  <si>
+    <t>300V</t>
   </si>
 </sst>
 </file>
@@ -486,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -501,7 +516,7 @@
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -529,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -540,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -549,6 +564,40 @@
       </c>
       <c r="E4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>41019</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>41019</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -563,10 +612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -681,6 +730,32 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>41026</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41026</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added new buck filtering test. 5-15
</commit_message>
<xml_diff>
--- a/capDatabase.xlsx
+++ b/capDatabase.xlsx
@@ -153,12 +153,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -179,9 +185,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -638,7 +646,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -753,29 +761,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
+    <row r="6" spans="1:8" s="3" customFormat="1">
+      <c r="A6" s="2">
         <v>41026</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>41026</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>